<commit_message>
working on market report
</commit_message>
<xml_diff>
--- a/application/plugins/Reports_market_analyse/Reports_market_analyse.xlsx
+++ b/application/plugins/Reports_market_analyse/Reports_market_analyse.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Название</t>
   </si>
@@ -73,29 +73,56 @@
     <t>Бренд</t>
   </si>
   <si>
-    <t>{$v-&gt;type_rows[]-&gt;sold}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;type_rows[]-&gt;sold_sum}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;type_rows[]-&gt;leftover}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;type_rows[]-&gt;leftover_sum}</t>
-  </si>
-  <si>
     <t>шт</t>
   </si>
   <si>
-    <t>{$v-&gt;type_rows[]-&gt;group_by}</t>
+    <t>{$v-&gt;rows[]-&gt;avg_price}</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>сумма</t>
+  </si>
+  <si>
+    <t>средняя</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum_rows[]-&gt;group_by}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum_rows[]-&gt;sold}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum_rows[]-&gt;sold_sum}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum_rows[]-&gt;leftover}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum_rows[]-&gt;leftover_sum}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum-&gt;sum_leftover_sum}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum-&gt;sum_sold_sum}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum-&gt;sum_leftover}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;sum-&gt;sum_sold}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#\ ##0_);\(#\ ##0\)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,15 +150,6 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -173,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -227,6 +245,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -234,7 +278,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -243,7 +289,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -254,7 +302,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -262,7 +312,9 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -271,7 +323,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -282,28 +336,17 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -319,92 +362,649 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -581,9 +1181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -621,9 +1221,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,7 +1258,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -693,7 +1293,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -867,195 +1467,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:N11"/>
+  <dimension ref="E2:O11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="2.28515625" customWidth="1"/>
-    <col min="5" max="9" width="10.28515625" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="35.5703125" customWidth="1"/>
-    <col min="11" max="14" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="15" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="J2" s="8" t="s">
+    <row r="2" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="28"/>
+    </row>
+    <row r="3" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+      <c r="L3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="5:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="L5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="5:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="36"/>
+    </row>
+    <row r="8" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="21" t="s">
+      <c r="M8" s="27"/>
+      <c r="N8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="22"/>
+      <c r="O8" s="33"/>
     </row>
-    <row r="3" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="5"/>
-      <c r="K3" s="29" t="s">
+    <row r="9" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="10"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="31"/>
+      <c r="L9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="5:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J4" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="32" t="s">
+    <row r="10" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>22</v>
+      <c r="L10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="5:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="20"/>
-    </row>
-    <row r="8" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="24"/>
-      <c r="M8" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="9" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E9" s="17"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="10"/>
-    </row>
-    <row r="10" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
+    <row r="11" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
+  <mergeCells count="6">
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="E11:O11"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="E7:O7"/>
   </mergeCells>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="J10:L10">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>